<commit_message>
fleet and work place scaled comparison graphs
</commit_message>
<xml_diff>
--- a/Model_Map/Fleet_Scaled_Comparison_Graphs.xlsx
+++ b/Model_Map/Fleet_Scaled_Comparison_Graphs.xlsx
@@ -16983,13 +16983,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH2:BN26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>

</xml_diff>